<commit_message>
Adding Properties All Changing Flight Flow
</commit_message>
<xml_diff>
--- a/FCMMBFlow/src/test/resources/TestData/TestData.xlsx
+++ b/FCMMBFlow/src/test/resources/TestData/TestData.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300"/>
+    <workbookView windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="MMBChangeDateSelection" sheetId="2" r:id="rId2"/>
+    <sheet name="MMBPaymentDetails" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
   <si>
     <t>Login Field</t>
   </si>
@@ -54,6 +56,153 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>BookingActions</t>
+  </si>
+  <si>
+    <t>Change Flight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMB method selection </t>
+  </si>
+  <si>
+    <t>Travel Selection for MMB ChangeFlight</t>
+  </si>
+  <si>
+    <t>Trip index</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Trip Selection for oneway OB =0, round trip IB only=1,roundtrip=2</t>
+  </si>
+  <si>
+    <t>OBSegmentMonth</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>Month of travel ----OB segemnt</t>
+  </si>
+  <si>
+    <t>OBSegmentDate</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>date of travel</t>
+  </si>
+  <si>
+    <t>OBSegmentYear</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>Year of travel</t>
+  </si>
+  <si>
+    <t>IBSegmentMonth</t>
+  </si>
+  <si>
+    <t>Month of travel ---- IB Segment</t>
+  </si>
+  <si>
+    <t>IBSegmentDate</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>IBSegmentYear</t>
+  </si>
+  <si>
+    <t>Cabin Fare Selection</t>
+  </si>
+  <si>
+    <t>Fare</t>
+  </si>
+  <si>
+    <t>Fare Selection like --pro,eco,bus,busfx</t>
+  </si>
+  <si>
+    <t>OB segemnt</t>
+  </si>
+  <si>
+    <t>pro</t>
+  </si>
+  <si>
+    <t>IB segemnt</t>
+  </si>
+  <si>
+    <t>Carddetails</t>
+  </si>
+  <si>
+    <t>Given Credit card details for booking MMB flow</t>
+  </si>
+  <si>
+    <t>CardNo</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>Card Type (Visa ,Master card )</t>
+  </si>
+  <si>
+    <t>CCV</t>
+  </si>
+  <si>
+    <t>Expirationyear</t>
+  </si>
+  <si>
+    <t>Expirationmonth</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Billingdetails</t>
+  </si>
+  <si>
+    <t>Provide Billing Data for booking</t>
+  </si>
+  <si>
+    <t>Tamil</t>
+  </si>
+  <si>
+    <t>GQ</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>25,SaiBaba</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Coimbatore</t>
+  </si>
+  <si>
+    <t>Postalcode</t>
+  </si>
+  <si>
+    <t>Mobile No</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -66,7 +215,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,28 +231,36 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -553,161 +710,183 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1029,58 +1208,419 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="12.7142857142857" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.2857142857143" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.4285714285714" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="12.7142857142857" style="10" customWidth="1"/>
+    <col min="2" max="2" width="12.2857142857143" style="10" customWidth="1"/>
+    <col min="3" max="3" width="12.4285714285714" style="10" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="39.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="65" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="10"/>
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="10"/>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="10"/>
+      <c r="C17" s="9"/>
+    </row>
+  </sheetData>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"Change Flight,Manage Seats &amp; Add-ons"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"0,1,2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B9">
+      <formula1>"January,February,March,April,May,June,July,August,September,October,November,December"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 B10">
+      <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8 B11">
+      <formula1>"2024,2025,2026,2027,2028,2029,2030"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4">
+      <formula1>"Change Flight"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B16">
+      <formula1>"pro,eco,bus,busfx"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="17.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="18.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="47.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="5">
+        <v>641001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="5">
+        <v>9876543210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"2024,2025,2026,2027,2028,2029,2030"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+      <formula1>"January,February,March,April,May,June,July,August,September,October,November,December"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>